<commit_message>
Corrected error in 2014 data Signed-off-by: Gerry Mulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/europarl/transfers.2014-05-22.xlsx
+++ b/europarl/transfers.2014-05-22.xlsx
@@ -913,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13:Q22"/>
+    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1638,12 +1638,12 @@
         <v>179302.53</v>
       </c>
       <c r="P18" s="3">
-        <f>156132-O18</f>
-        <v>-23170.53</v>
+        <f>156532-O18</f>
+        <v>-22770.53</v>
       </c>
       <c r="Q18" s="3">
         <f t="shared" si="0"/>
-        <v>156132</v>
+        <v>156532</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>